<commit_message>
model set up with parallel processing
</commit_message>
<xml_diff>
--- a/ScenarioGuide.xlsx
+++ b/ScenarioGuide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\IFsCore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\BIGPOPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0FC192-CC66-40CB-862E-3B806FE4652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9DEDD6-4116-4C2C-9A68-C8098ED8E43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="732" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{EDC72DCC-50B8-433C-A59E-5BD754D82CFC}"/>
+    <workbookView xWindow="1368" yWindow="1620" windowWidth="19176" windowHeight="10284" xr2:uid="{EDC72DCC-50B8-433C-A59E-5BD754D82CFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Para_Demo_Global" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Coef_Demo_Global!$A$1:$J$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Para_Demo_Global!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Var_Output!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Var_Output!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -300,12 +300,45 @@
   </si>
   <si>
     <t>AnalysisSwitch</t>
+  </si>
+  <si>
+    <t>HistTable</t>
+  </si>
+  <si>
+    <t>Total Number of CPUs (# of Model Runs in Parallel)</t>
+  </si>
+  <si>
+    <t>SeriesPopulation</t>
+  </si>
+  <si>
+    <t>SeriesTFR</t>
+  </si>
+  <si>
+    <t>SeriesLifeExpectIHMEBothSexesHistOnly</t>
+  </si>
+  <si>
+    <t>SeriesForecastBirthsMedUNPD</t>
+  </si>
+  <si>
+    <t>SeriesDeathsper1000IHMEForecasts</t>
+  </si>
+  <si>
+    <t>CompareSwitch</t>
+  </si>
+  <si>
+    <t>Total Estimated Time (Hours)</t>
+  </si>
+  <si>
+    <t>Mins per Model Run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,8 +368,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB9080E-D106-45C5-9A08-BCC54809119D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +769,7 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -778,7 +813,7 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
@@ -807,10 +842,10 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
@@ -830,7 +865,7 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1273,12 +1308,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85E024F-DC0A-435E-AA73-F3BC460E3BD6}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="4" width="11.44140625" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
@@ -1344,10 +1380,10 @@
         <v>1.09E-2</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1.09E-2</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1373,13 +1409,13 @@
         <v>-0.8327</v>
       </c>
       <c r="H3">
-        <v>-2</v>
+        <v>-0.8327</v>
       </c>
       <c r="I3">
-        <v>0.01</v>
+        <v>-0.8327</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1405,13 +1441,13 @@
         <v>-9.4800000000000006E-3</v>
       </c>
       <c r="H4">
-        <v>-1.4999999999999999E-2</v>
+        <v>-9.4800000000000006E-3</v>
       </c>
       <c r="I4">
-        <v>-1E-3</v>
+        <v>-9.4800000000000006E-3</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1523,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6160BC4B-9AFF-4BF2-A9D5-14191B7561B6}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,9 +1570,11 @@
     <col min="1" max="1" width="19.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.109375" customWidth="1"/>
     <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1546,8 +1584,14 @@
       <c r="C1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1557,8 +1601,14 @@
       <c r="C2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1568,8 +1618,14 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1579,8 +1635,14 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1590,8 +1652,14 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1601,11 +1669,17 @@
       <c r="C6" t="s">
         <v>37</v>
       </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C6" xr:uid="{6160BC4B-9AFF-4BF2-A9D5-14191B7561B6}"/>
+  <autoFilter ref="A1:E6" xr:uid="{6160BC4B-9AFF-4BF2-A9D5-14191B7561B6}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{6C2EBF5B-C834-4EEE-8E31-8F76517BD517}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6 E2:E7" xr:uid="{6C2EBF5B-C834-4EEE-8E31-8F76517BD517}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1616,33 +1690,59 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26476899-C05F-4187-8710-D2A6E0F6A2E0}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" cm="1">
+      <c r="B1" s="2" cm="1">
         <f t="array" ref="B1">PRODUCT(IF(Coef_Demo_Global!F2:F19="On", Coef_Demo_Global!J2:J19, 1))*PRODUCT(IF(Para_Demo_Global!E2:E19="On", Para_Demo_Global!I2:I19, 1))</f>
-        <v>3888</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B2">
-        <f>B1*360/(60*60*24)</f>
-        <v>16.2</v>
+      <c r="B4" s="1">
+        <f>(B1*(B2*60)/(60*60*24))/B3</f>
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4*24</f>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>